<commit_message>
Updated app to fix invite last sent date
</commit_message>
<xml_diff>
--- a/template2.xlsx
+++ b/template2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loftu\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loftu\Desktop\EverbrightApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048CA0C0-B4D7-4191-B64E-549446B10821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063DAB96-45B8-4441-8B18-621116460461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" tabRatio="629" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>Total users:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Finished:</t>
   </si>
@@ -64,6 +61,15 @@
   <si>
     <t>COURSE NAME</t>
   </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CORR </t>
+  </si>
+  <si>
+    <t>USER PROGRESS REPORT</t>
+  </si>
 </sst>
 </file>
 
@@ -72,7 +78,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -232,8 +238,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="35">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -425,8 +439,20 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEC0E4D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -491,32 +517,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -629,27 +629,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -675,49 +739,63 @@
     <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="36" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="35" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -771,7 +849,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -779,7 +857,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -787,7 +865,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -795,7 +873,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -803,7 +881,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -811,7 +889,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -819,7 +897,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -867,15 +945,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="B12:G13" insertRow="1" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="B12:G13" insertRow="1" totalsRowShown="0" headerRowDxfId="7" dataDxfId="0">
   <autoFilter ref="B12:G13" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="USER" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="EMAIL" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="COURSE NAME" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="STATUS" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{36817819-12DD-4004-A744-A40880192678}" name="DATE" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{EE70BA52-D738-4000-99CE-FF994A857A90}" name="SCORE" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="USER" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="EMAIL" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="COURSE NAME" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="STATUS" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{36817819-12DD-4004-A744-A40880192678}" name="DATE" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{EE70BA52-D738-4000-99CE-FF994A857A90}" name="SCORE" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1184,188 +1262,245 @@
   <dimension ref="B1:G42"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:G13"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="9.15625" style="1"/>
-    <col min="2" max="2" width="19.3125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7890625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.20703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83984375" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.47265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.1015625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7890625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5234375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.20703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.83984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.47265625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9.15625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-    </row>
-    <row r="2" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="10">
+    <row r="1" spans="2:7" ht="20.399999999999999" x14ac:dyDescent="0.75">
+      <c r="B1" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="18"/>
+    </row>
+    <row r="2" spans="2:7" ht="20.7" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="B2" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="20"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3" s="27"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="21"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" s="30">
         <f ca="1">TODAY()</f>
-        <v>45636</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="3" t="s">
+        <v>45638</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="22"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" s="26"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="22"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="31">
+        <f>COUNTIF(E:E,"Passed")</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="22"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="31">
+        <f>COUNTIF(E:E,"In Progress")</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="22"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="31">
+        <f>COUNTIF(E:E,"Not Started")</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="22"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="31">
+        <f>SUM(C6:C8)</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="22"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" s="25"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="24"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="4">
-        <f ca="1">COUNTIF(C:C,"Passed")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="5" t="s">
+      <c r="C12" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="6">
-        <f ca="1">COUNTIF(C:C,"In Progress")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="8">
-        <f ca="1">COUNTIF(C:C,"Not Started")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="2"/>
-      <c r="C7" s="15"/>
-    </row>
-    <row r="8" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="9">
-        <f ca="1">SUM(C4:C6)</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F10" s="1"/>
-    </row>
-    <row r="12" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="11" t="s">
+      <c r="G12" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F12" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="6:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="6:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="6:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="6:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="6:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="6:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="6:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="6:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="6:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="6:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="6:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="6:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="6:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="6:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="6:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="6:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="6:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F33" s="1"/>
-    </row>
-    <row r="34" spans="6:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F34" s="1"/>
-    </row>
-    <row r="35" spans="6:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F35" s="1"/>
-    </row>
-    <row r="36" spans="6:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F36" s="1"/>
-    </row>
-    <row r="37" spans="6:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F37" s="1"/>
-    </row>
-    <row r="38" spans="6:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F38" s="1"/>
-    </row>
-    <row r="39" spans="6:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F39" s="1"/>
-    </row>
-    <row r="40" spans="6:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F40" s="1"/>
-    </row>
-    <row r="41" spans="6:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F41" s="1"/>
-    </row>
-    <row r="42" spans="6:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F42" s="1"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F33" s="2"/>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F37" s="2"/>
+    </row>
+    <row r="38" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F38" s="2"/>
+    </row>
+    <row r="39" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F39" s="2"/>
+    </row>
+    <row r="40" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F40" s="2"/>
+    </row>
+    <row r="41" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F41" s="2"/>
+    </row>
+    <row r="42" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F42" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Initial commit for NewReportApp
</commit_message>
<xml_diff>
--- a/template2.xlsx
+++ b/template2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loftu\Desktop\EverbrightApp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loftu\Desktop\NewReportApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063DAB96-45B8-4441-8B18-621116460461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF4FE60-DA6D-4F6F-B649-D47D54AC1BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" tabRatio="629" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -739,23 +739,18 @@
     <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="36" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -849,7 +844,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -857,7 +852,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -865,7 +860,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -873,7 +868,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -881,7 +876,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -889,7 +884,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -897,7 +892,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1262,245 +1257,237 @@
   <dimension ref="B1:G42"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="9.15625" style="1"/>
-    <col min="2" max="2" width="30.1015625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7890625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5234375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.20703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.47265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.1015625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7890625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.20703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.83984375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.47265625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9.15625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="18"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="2:7" ht="20.7" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="16" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="20"/>
+      <c r="G2" s="17"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="27"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="21"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="18"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="30">
+      <c r="B4" s="27">
         <f ca="1">TODAY()</f>
         <v>45638</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="22"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="19"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="26"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="22"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="19"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="31">
+      <c r="C6" s="28">
         <f>COUNTIF(E:E,"Passed")</f>
         <v>0</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="22"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="19"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="31">
+      <c r="C7" s="28">
         <f>COUNTIF(E:E,"In Progress")</f>
         <v>0</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="22"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="19"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="31">
+      <c r="C8" s="28">
         <f>COUNTIF(E:E,"Not Started")</f>
         <v>0</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="22"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="19"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="31">
+      <c r="C9" s="28">
         <f>SUM(C6:C8)</f>
         <v>0</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="22"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="19"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10" s="25"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="24"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="8"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="G12" s="10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F13" s="2"/>
+      <c r="F13" s="1"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F14" s="2"/>
+      <c r="F14" s="1"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F15" s="2"/>
+      <c r="F15" s="1"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F16" s="2"/>
+      <c r="F16" s="1"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F17" s="2"/>
+      <c r="F17" s="1"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F18" s="2"/>
+      <c r="F18" s="1"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F19" s="2"/>
+      <c r="F19" s="1"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F20" s="2"/>
+      <c r="F20" s="1"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F21" s="2"/>
+      <c r="F21" s="1"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F22" s="2"/>
+      <c r="F22" s="1"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F23" s="2"/>
+      <c r="F23" s="1"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F24" s="2"/>
+      <c r="F24" s="1"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F25" s="2"/>
+      <c r="F25" s="1"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F26" s="2"/>
+      <c r="F26" s="1"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F27" s="2"/>
+      <c r="F27" s="1"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F28" s="2"/>
+      <c r="F28" s="1"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F29" s="2"/>
+      <c r="F29" s="1"/>
     </row>
     <row r="30" spans="6:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F30" s="2"/>
+      <c r="F30" s="1"/>
     </row>
     <row r="31" spans="6:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F31" s="2"/>
+      <c r="F31" s="1"/>
     </row>
     <row r="32" spans="6:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F32" s="2"/>
+      <c r="F32" s="1"/>
     </row>
     <row r="33" spans="6:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F33" s="2"/>
+      <c r="F33" s="1"/>
     </row>
     <row r="34" spans="6:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F34" s="2"/>
+      <c r="F34" s="1"/>
     </row>
     <row r="35" spans="6:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F35" s="2"/>
+      <c r="F35" s="1"/>
     </row>
     <row r="36" spans="6:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F36" s="2"/>
+      <c r="F36" s="1"/>
     </row>
     <row r="37" spans="6:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F37" s="2"/>
+      <c r="F37" s="1"/>
     </row>
     <row r="38" spans="6:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F38" s="2"/>
+      <c r="F38" s="1"/>
     </row>
     <row r="39" spans="6:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F39" s="2"/>
+      <c r="F39" s="1"/>
     </row>
     <row r="40" spans="6:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F40" s="2"/>
+      <c r="F40" s="1"/>
     </row>
     <row r="41" spans="6:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F41" s="2"/>
+      <c r="F41" s="1"/>
     </row>
     <row r="42" spans="6:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F42" s="2"/>
+      <c r="F42" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>